<commit_message>
added excel file changes
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ara Alepoghelian\Desktop\passwordGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ara Alepoghelian\Desktop\passwordgenpy\passwordgenerator-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{804BF007-BB15-4634-80FC-71C782DC3281}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5500EB-4789-44DB-84ED-5AA59EA19114}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16260" xr2:uid="{C7081CE2-E821-4EB4-93B3-F6BC4A1A6044}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pass" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>